<commit_message>
Actualizado desde bases publicas. Pendiente correr factorial de nuevo.
</commit_message>
<xml_diff>
--- a/Output/BBDD/tablas descriptivas.xlsx
+++ b/Output/BBDD/tablas descriptivas.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -395,12 +395,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>a64rec</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Meses desemplado año anterior</t>
+          <t>T1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -434,27 +429,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>a21</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Percepción de estabilidad del empleo</t>
+          <t>T2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Mean (sd) : 2 (0.8)\
-min &lt; med &lt; max:\
-1 &lt; 2 &lt; 3\
-IQR (CV) : 2 (0.4)</t>
+          <t>Mean (sd) : 1 (0.8)\
+min &lt; med &lt; max:\
+0 &lt; 1 &lt; 2\
+IQR (CV) : 2 (0.8)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1 : 669 (31.6%)\
-2 : 743 (35.1%)\
-3 : 703 (33.2%)</t>
+          <t>0 : 669 (31.6%)\
+1 : 743 (35.1%)\
+2 : 703 (33.2%)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -470,25 +460,20 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>a22</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Trabajo permanente o de temporada</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Min  : 1\
-Mean : 1.1\
-Max  : 2</t>
+          <t>Min  : 0\
+Mean : 0.1\
+Max  : 1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1 : 1811 (85.6%)\
-2 :  304 (14.4%)</t>
+          <t>0 : 1811 (85.6%)\
+1 :  304 (14.4%)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -504,12 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>a23rec</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Años en el actual trabajo</t>
+          <t>T4</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -542,12 +522,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>a48rec</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Tramo de ingresos líquidos percibidos por el trabajo</t>
+          <t>I1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -580,12 +555,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>a50rec</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Cobertura de necesidades básicas por ingresos del trabajo</t>
+          <t>I2</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -618,12 +588,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>a50arec</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Cobertura de imprevistos por ingresos del trabajo</t>
+          <t>I3</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -656,27 +621,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>a70rec</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Pensión (afiliado y cotiza)</t>
+          <t>D1</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Mean (sd) : 3.1 (14.8)\
-min &lt; med &lt; max:\
-0 &lt; 1 &lt; 99\
-IQR (CV) : 0 (4.8)</t>
+          <t>Mean (sd) : 0.9 (0.4)\
+min &lt; med &lt; max:\
+0 &lt; 1 &lt; 2\
+IQR (CV) : 0 (0.5)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0  :  351 (16.6%)\
-1  : 1715 (81.1%)\
-99 :   49 ( 2.3%)</t>
+          <t>0 :  351 (16.6%)\
+1 : 1715 (81.1%)\
+2 :   49 ( 2.3%)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -692,27 +652,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>a73rec</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Seguro de cesantía</t>
+          <t>D2</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Mean (sd) : 4.1 (17.2)\
-min &lt; med &lt; max:\
-0 &lt; 1 &lt; 99\
-IQR (CV) : 0 (4.2)</t>
+          <t>Mean (sd) : 1 (0.3)\
+min &lt; med &lt; max:\
+0 &lt; 1 &lt; 2\
+IQR (CV) : 0 (0.3)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0  :   86 ( 4.1%)\
-1  : 1962 (92.8%)\
-99 :   67 ( 3.2%)</t>
+          <t>0 :   86 ( 4.1%)\
+1 : 1962 (92.8%)\
+2 :   67 ( 3.2%)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -728,27 +683,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>salud</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Pensión (cotiza o carga)</t>
+          <t>D3</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Mean (sd) : 2.8 (12.5)\
-min &lt; med &lt; max:\
-1 &lt; 1 &lt; 99\
-IQR (CV) : 0 (4.5)</t>
+          <t>Mean (sd) : 0.2 (0.4)\
+min &lt; med &lt; max:\
+0 &lt; 0 &lt; 2\
+IQR (CV) : 0 (2.4)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1  : 1785 (84.4%)\
-2  :  295 (14.0%)\
-99 :   35 ( 1.6%)</t>
+          <t>0 : 1785 (84.4%)\
+1 :  295 (14.0%)\
+2 :   35 ( 1.6%)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -764,12 +714,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>a67arec</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Días feriados</t>
+          <t>E1</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -802,12 +747,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>a67brec</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Uso de licencia o reposo</t>
+          <t>E2</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -840,12 +780,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>a67crec</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Ir al médico</t>
+          <t>E3</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -878,12 +813,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>a67drec</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Tomar las vacaciones</t>
+          <t>E4</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -916,12 +846,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>a67erec</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Día libre</t>
+          <t>E5</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -954,25 +879,20 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>a32rec</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Encadenamiento a clientes</t>
+          <t>CEX1</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Min  : 1\
-Mean : 1.1\
-Max  : 2</t>
+          <t>Min  : 0\
+Mean : 0.1\
+Max  : 1</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1 : 1814 (85.8%)\
-2 :  301 (14.2%)</t>
+          <t>0 : 1814 (85.8%)\
+1 :  301 (14.2%)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -988,28 +908,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>a33rec</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Encadenamiento proveedores</t>
+          <t>CEX2</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Mean (sd) : 1.6 (0.9)\
-min &lt; med &lt; max:\
-1 &lt; 1 &lt; 4\
-IQR (CV) : 1 (0.6)</t>
+          <t>Mean (sd) : 0.5 (0.7)\
+min &lt; med &lt; max:\
+0 &lt; 0 &lt; 2\
+IQR (CV) : 1 (1.3)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1 : 1225 (57.9%)\
-2 :  633 (29.9%)\
-3 :   71 ( 3.4%)\
-4 :  186 ( 8.8%)</t>
+          <t>0 : 1225 (57.9%)\
+1 :  633 (29.9%)\
+2 :  257 (12.2%)</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1025,25 +939,20 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>a34rec</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>¿Tiene algún tipo de contrato, acuerdo o compromiso con su cliente y/o proveedor?</t>
+          <t>CEX3</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Min  : 1\
-Mean : 1.2\
-Max  : 2</t>
+          <t>Min  : 0\
+Mean : 0.1\
+Max  : 1</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1 : 1725 (81.6%)\
-2 :  390 (18.4%)</t>
+          <t>0 : 1842 (87.1%)\
+1 :  273 (12.9%)</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1059,25 +968,20 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>a35rec</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Normatividad del trabajo por cliente o proveedor</t>
+          <t>CEX4</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Min  : 1\
-Mean : 1.1\
-Max  : 2</t>
+          <t>Min  : 0\
+Mean : 0.1\
+Max  : 1</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1 : 1842 (87.1%)\
-2 :  273 (12.9%)</t>
+          <t>0 : 1968 (93.0%)\
+1 :  147 ( 7.0%)</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1093,25 +997,20 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>a36rec</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Exclusividad exigida por cliente o proveedor</t>
+          <t>CEN1</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Min  : 1\
-Mean : 1.1\
-Max  : 2</t>
+          <t>Min  : 0\
+Mean : 0.3\
+Max  : 1</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1 : 1968 (93.0%)\
-2 :  147 ( 7.0%)</t>
+          <t>0 : 1379 (65.2%)\
+1 :  736 (34.8%)</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1127,33 +1026,20 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>subempleo</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Horas promedio no trabajadas la semana pasada bajo las 8 horas</t>
+          <t>CEN2</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Mean (sd) : 4 (14.4)\
-min &lt; med &lt; max:\
-1 &lt; 1 &lt; 99\
-IQR (CV) : 2 (3.6)</t>
+          <t>Min  : 0\
+Mean : 0.8\
+Max  : 1</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1  : 1408 (66.6%)\
-2  :  124 ( 5.9%)\
-3  :  203 ( 9.6%)\
-4  :  156 ( 7.4%)\
-5  :  107 ( 5.1%)\
-6  :   40 ( 1.9%)\
-7  :   22 ( 1.0%)\
-8  :    8 ( 0.4%)\
-99 :   47 ( 2.2%)</t>
+          <t>0 :  376 (17.8%)\
+1 : 1739 (82.2%)</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1169,25 +1055,20 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>sobretrabajo</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Horas diarias por sobre la jornada de ocho horas</t>
+          <t>CEN3</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Mean (sd) : 3.6 (14.6)\
-min &lt; med &lt; max:\
-0 &lt; 0 &lt; 99\
-IQR (CV) : 2 (4)</t>
+          <t>Min  : 0\
+Mean : 0.5\
+Max  : 1</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>14 distinct values</t>
+          <t>0 : 1140 (53.9%)\
+1 :  975 (46.1%)</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1203,100 +1084,28 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>a42</t>
+          <t>FEXP_MAY15</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Horas trabajadas los sábados</t>
+          <t>FACTOR EXPANSIÓN</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Mean (sd) : 6.4 (4.1)\
-min &lt; med &lt; max:\
-0 &lt; 7 &lt; 20\
-IQR (CV) : 5 (0.6)</t>
+          <t>Mean (sd) : 726.6 (1455.6)\
+min &lt; med &lt; max:\
+4.8 &lt; 307.1 &lt; 20920.1\
+IQR (CV) : 628.1 (2)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>21 distinct values</t>
+          <t>1747 distinct values</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
-        <is>
-          <t>0\
-(0%)</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>a43</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Horas trabajadas los domingos</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Mean (sd) : 3.4 (4.3)\
-min &lt; med &lt; max:\
-0 &lt; 0 &lt; 20\
-IQR (CV) : 6 (1.3)</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>21 distinct values</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>0\
-(0%)</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>a44</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Domingos trabajados al mes</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Mean (sd) : 2.7 (1.7)\
-min &lt; med &lt; max:\
-1 &lt; 2 &lt; 5\
-IQR (CV) : 4 (0.7)</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>1 : 970 (45.9%)\
-2 : 144 ( 6.8%)\
-3 : 266 (12.6%)\
-4 : 121 ( 5.7%)\
-5 : 614 (29.0%)</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
         <is>
           <t>0\
 (0%)</t>

</xml_diff>